<commit_message>
bug fixes chrome extension
</commit_message>
<xml_diff>
--- a/data/product recommendation query set.xlsx
+++ b/data/product recommendation query set.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\OneDrive\Desktop\Thesis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\OneDrive\Desktop\Search vs Generation - A Comparative Study of Bing and ChatGPT in Product Recommendations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56672BD5-C20A-431C-8241-EEC352A410C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5368C712-E5B2-48D8-B11E-8EA1106D4E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13210" yWindow="2040" windowWidth="21900" windowHeight="15380" xr2:uid="{B28B15D7-B92C-4996-AB7A-16FAE932B28F}"/>
+    <workbookView xWindow="11660" yWindow="3770" windowWidth="21900" windowHeight="15380" xr2:uid="{B28B15D7-B92C-4996-AB7A-16FAE932B28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -623,7 +623,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>